<commit_message>
[IMP] Adjust Payable Balance Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_payable_balance.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_payable_balance.xlsx
@@ -20,15 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t xml:space="preserve">รายงานสถานะเจ้าหนี้</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Payable Balance Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Code</t>
   </si>
   <si>
     <t xml:space="preserve">Supplier</t>
   </si>
   <si>
-    <t xml:space="preserve">Account Code</t>
+    <t xml:space="preserve">Fiscal Year From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date To</t>
   </si>
   <si>
     <t xml:space="preserve">Run By</t>
@@ -68,10 +89,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#,###.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -99,6 +122,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -155,25 +184,49 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -201,10 +254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -215,75 +268,113 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="30.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="28.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="26.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="26.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="4" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="8" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="C12" s="11" t="s">
         <v>13</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>